<commit_message>
final code dus klaar voor voorspelling
</commit_message>
<xml_diff>
--- a/Forecasts_By_Window/Forecast_Window_1.xlsx
+++ b/Forecasts_By_Window/Forecast_Window_1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,208 +463,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DTPQ67872X</t>
+          <t>merged_06GE2U92FA_DTPQ67872X_G8WP29EHC6_HYT3MYM7CY_IMFA21HLV3_JU9OS20S99_PPB56V08LB_R5X6KPETN3_RX38XS00QN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>onesize</t>
+          <t>merged_L_M_S_XL_XS_XXL_XXS_onesize</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Platform</t>
+          <t>merged_Amsterdam_Berlin_Brussels_Copenhagen_Helsinki_Madrid_Paris_Platform_Rome_Stockholm_Webshop</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>2024</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>DTPQ67872X</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>onesize</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Webshop</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E3" t="n">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DTPQ67872X</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>onesize</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>merged_Amsterdam_Berlin_Brussels_Copenhagen_Helsinki_Madrid_Paris_Rome_Stockholm</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E4" t="n">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RX38XS00QN</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Platform</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E5" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>RX38XS00QN</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Webshop</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E6" t="n">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>RX38XS00QN</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>merged_Amsterdam_Berlin_Brussels_Copenhagen_Helsinki_Madrid_Paris_Rome_Stockholm</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E7" t="n">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>merged_06GE2U92FA_G8WP29EHC6_HYT3MYM7CY_IMFA21HLV3_JU9OS20S99_PPB56V08LB_R5X6KPETN3</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Platform</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E8" t="n">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>merged_06GE2U92FA_G8WP29EHC6_HYT3MYM7CY_IMFA21HLV3_JU9OS20S99_PPB56V08LB_R5X6KPETN3</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Webshop</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2571</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>merged_06GE2U92FA_G8WP29EHC6_HYT3MYM7CY_IMFA21HLV3_JU9OS20S99_PPB56V08LB_R5X6KPETN3</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>merged_L_M_S_XL_XS_XXL_XXS</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>merged_Amsterdam_Berlin_Brussels_Copenhagen_Helsinki_Madrid_Paris_Rome_Stockholm</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>2024</v>
-      </c>
-      <c r="E10" t="n">
-        <v>8768</v>
+        <v>12651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>